<commit_message>
AA SSO automatic handling
</commit_message>
<xml_diff>
--- a/CucumberCraft/target/test-classes/Fixture/Promo_DB_Data.xlsx
+++ b/CucumberCraft/target/test-classes/Fixture/Promo_DB_Data.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -142,9 +141,6 @@
     <t>TestId</t>
   </si>
   <si>
-    <t>https://apt-dev.apps.depaas.qcorpaa.aa.com/</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -383,6 +379,9 @@
   </si>
   <si>
     <t>Verify the pagination is absent</t>
+  </si>
+  <si>
+    <t>https://apt-qa.apps.sepaas.aa.com</t>
   </si>
 </sst>
 </file>
@@ -815,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,25 +842,25 @@
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="K1" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L1" s="8"/>
     </row>
@@ -876,7 +875,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -899,7 +898,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -922,7 +921,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -942,10 +941,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -968,10 +967,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -993,10 +992,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1018,10 +1017,10 @@
         <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1043,10 +1042,10 @@
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1068,10 +1067,10 @@
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1093,10 +1092,10 @@
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1118,10 +1117,10 @@
         <v>30</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1143,10 +1142,10 @@
         <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1168,10 +1167,10 @@
         <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1193,10 +1192,10 @@
         <v>33</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1218,10 +1217,10 @@
         <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1243,10 +1242,10 @@
         <v>35</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1268,10 +1267,10 @@
         <v>36</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1293,10 +1292,10 @@
         <v>37</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1309,19 +1308,19 @@
     </row>
     <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F20" s="3" t="str">
         <f>CONCATENATE("https://lscs-tst-adv.qcorpaa.aa.com/lscs-static/324/242/3242429b7935f62252338ef8f41d1745/content/pubcontent/en_US/aadvantage-promotions/promotion/",E20,".json")</f>
@@ -1337,19 +1336,19 @@
     </row>
     <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" s="3" t="str">
         <f>CONCATENATE("https://lscs-tst-adv.qcorpaa.aa.com/lscs-static/324/242/3242429b7935f62252338ef8f41d1745/content/pubcontent/en_US/aadvantage-promotions/promotion/",E21,".json")</f>
@@ -1365,19 +1364,19 @@
     </row>
     <row r="22" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="3" t="str">
         <f t="shared" ref="F22" si="0">CONCATENATE("https://lscs-tst-adv.qcorpaa.aa.com/lscs-static/324/242/3242429b7935f62252338ef8f41d1745/content/pubcontent/en_US/aadvantage-promotions/promotion/",E22,".json")</f>
@@ -1393,19 +1392,19 @@
     </row>
     <row r="23" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" s="3" t="str">
         <f>CONCATENATE("https://lscs-tst-adv.qcorpaa.aa.com/lscs-static/324/242/3242429b7935f62252338ef8f41d1745/content/pubcontent/en_US/aadvantage-promotions/promotion/","RVGLD",".json")</f>
@@ -1421,19 +1420,19 @@
     </row>
     <row r="24" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="F24" s="3" t="str">
         <f>CONCATENATE("https://lscs-tst-adv.qcorpaa.aa.com/lscs-static/324/242/3242429b7935f62252338ef8f41d1745/content/pubcontent/en_US/aadvantage-promotions/promotion/",E24,".json")</f>
@@ -1449,19 +1448,19 @@
     </row>
     <row r="25" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="3" t="str">
         <f t="shared" ref="F25:F30" si="1">CONCATENATE("https://lscs-tst-adv.qcorpaa.aa.com/lscs-static/324/242/3242429b7935f62252338ef8f41d1745/content/pubcontent/en_US/aadvantage-promotions/promotion/",E25,".json")</f>
@@ -1477,19 +1476,19 @@
     </row>
     <row r="26" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1505,19 +1504,19 @@
     </row>
     <row r="27" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F27" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1533,19 +1532,19 @@
     </row>
     <row r="28" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F28" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1561,19 +1560,19 @@
     </row>
     <row r="29" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F29" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1589,19 +1588,19 @@
     </row>
     <row r="30" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="3" t="str">
         <f t="shared" si="1"/>
@@ -1617,19 +1616,19 @@
     </row>
     <row r="31" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1642,16 +1641,16 @@
     </row>
     <row r="32" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="1"/>
@@ -1665,28 +1664,28 @@
     </row>
     <row r="33" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="F33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="H33" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1696,28 +1695,28 @@
     </row>
     <row r="34" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1727,53 +1726,53 @@
     </row>
     <row r="35" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I35" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="J35" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="K35" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L35" s="13"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1787,16 +1786,16 @@
     </row>
     <row r="37" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1810,16 +1809,16 @@
     </row>
     <row r="38" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1833,16 +1832,16 @@
     </row>
     <row r="39" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1856,34 +1855,34 @@
     </row>
     <row r="40" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>111</v>
-      </c>
       <c r="J40" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -1891,53 +1890,53 @@
     </row>
     <row r="41" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="D42" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" t="s">
         <v>117</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>120</v>
-      </c>
       <c r="D43" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>